<commit_message>
Maj Design Romain task
</commit_message>
<xml_diff>
--- a/Objectif/Objectif.xlsx
+++ b/Objectif/Objectif.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>DESIGN</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>Slide movement (Vector)</t>
+  </si>
+  <si>
+    <t>Design bumper (Generic)</t>
+  </si>
+  <si>
+    <t>Design platform (Generic)</t>
+  </si>
+  <si>
+    <t>Background music 1 (Paper)</t>
+  </si>
+  <si>
+    <t>Background music 2 (Paper)</t>
   </si>
 </sst>
 </file>
@@ -174,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,11 +209,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -210,8 +235,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +558,7 @@
     <col min="7" max="7" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -563,7 +589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -572,46 +598,48 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>7</v>
       </c>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>17</v>
       </c>
@@ -620,40 +648,42 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
         <v>20</v>
       </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>25</v>
       </c>
@@ -662,83 +692,115 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
         <v>28</v>
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>3</v>
       </c>
       <c r="G27" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
         <v>30</v>
       </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
         <v>31</v>
       </c>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
         <v>32</v>
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
         <v>33</v>
       </c>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
         <v>34</v>
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
         <v>35</v>
       </c>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
         <v>36</v>
       </c>
       <c r="H34" s="6"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>38</v>
+      </c>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>40</v>
+      </c>
+      <c r="H39" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Objectifs mis à jour
</commit_message>
<xml_diff>
--- a/Objectif/Objectif.xlsx
+++ b/Objectif/Objectif.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>DESIGN</t>
   </si>
@@ -139,6 +139,51 @@
   </si>
   <si>
     <t>Background music 2 (Paper)</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Auteur</t>
+  </si>
+  <si>
+    <t>Objectif</t>
+  </si>
+  <si>
+    <t>Stanislas</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Bases du moteur de jeu (Saut, collisions basiques)</t>
+  </si>
+  <si>
+    <t>Création d'une caméra sur rails</t>
+  </si>
+  <si>
+    <t>Jerome</t>
+  </si>
+  <si>
+    <t>Gestion fine des collisions</t>
+  </si>
+  <si>
+    <t>Implementation du saut mural</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Implementation des collectibles</t>
+  </si>
+  <si>
+    <t>Implementation du mouvement Glissade</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -226,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -238,6 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,20 +855,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>41920</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Objectifs mis à jour"
This reverts commit c6fe535d6862ad22a90624518c8e9763a5144493.
</commit_message>
<xml_diff>
--- a/Objectif/Objectif.xlsx
+++ b/Objectif/Objectif.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>DESIGN</t>
   </si>
@@ -139,51 +139,6 @@
   </si>
   <si>
     <t>Background music 2 (Paper)</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Auteur</t>
-  </si>
-  <si>
-    <t>Objectif</t>
-  </si>
-  <si>
-    <t>Stanislas</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Bases du moteur de jeu (Saut, collisions basiques)</t>
-  </si>
-  <si>
-    <t>Création d'une caméra sur rails</t>
-  </si>
-  <si>
-    <t>Jerome</t>
-  </si>
-  <si>
-    <t>Gestion fine des collisions</t>
-  </si>
-  <si>
-    <t>Implementation du saut mural</t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>Implementation des collectibles</t>
-  </si>
-  <si>
-    <t>Implementation du mouvement Glissade</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -271,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -283,7 +238,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,95 +809,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>41920</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last Maj design task
</commit_message>
<xml_diff>
--- a/Objectif/Objectif.xlsx
+++ b/Objectif/Objectif.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>DESIGN</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Design breakable (Paper)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hit lvl 1 (Vector) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hit lvl 1 (Generic) </t>
   </si>
 </sst>
 </file>
@@ -611,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,44 +887,56 @@
       </c>
       <c r="H41" s="6"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>68</v>
+      </c>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>69</v>
+      </c>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
         <v>41</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G46" t="s">
         <v>27</v>
       </c>
-      <c r="H44" s="8"/>
-    </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G45" t="s">
-        <v>28</v>
-      </c>
-      <c r="H45" s="6"/>
-    </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G46" t="s">
-        <v>42</v>
-      </c>
-      <c r="H46" s="6"/>
+      <c r="H46" s="8"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H47" s="6"/>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
+        <v>43</v>
+      </c>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>44</v>
+      </c>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
         <v>67</v>
       </c>
-      <c r="H49" s="6"/>
+      <c r="H51" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Chute ralenti contre mur
La chute en glissant contre un mur est ralenti
</commit_message>
<xml_diff>
--- a/Objectif/Objectif.xlsx
+++ b/Objectif/Objectif.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1131,7 @@
       <c r="G22" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="6"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" t="s">

</xml_diff>

<commit_message>
MAJ objectif + draft pos2
</commit_message>
<xml_diff>
--- a/Objectif/Objectif.xlsx
+++ b/Objectif/Objectif.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
   <si>
     <t>DESIGN</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>Background music 1 (Paper)</t>
-  </si>
-  <si>
-    <t>Background music 2 (Paper)</t>
   </si>
   <si>
     <t xml:space="preserve">Yuxing </t>
@@ -646,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +846,7 @@
       <c r="G30" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="6"/>
+      <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
@@ -882,7 +879,7 @@
       <c r="G36" t="s">
         <v>23</v>
       </c>
-      <c r="H36" s="6"/>
+      <c r="H36" s="5"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
@@ -910,7 +907,7 @@
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="H41" s="6"/>
     </row>
@@ -920,15 +917,9 @@
       </c>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G43" t="s">
-        <v>69</v>
-      </c>
-      <c r="H43" s="6"/>
-    </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G46" t="s">
         <v>27</v>
@@ -943,25 +934,25 @@
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H49" s="6"/>
     </row>
     <row r="50" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H50" s="6"/>
     </row>
     <row r="51" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H51" s="6"/>
     </row>
@@ -990,16 +981,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1007,79 +998,79 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
         <v>60</v>
       </c>
-      <c r="H3" t="s">
-        <v>61</v>
-      </c>
       <c r="J3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="5"/>
       <c r="J5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H7" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" s="6"/>
       <c r="J12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" s="6"/>
       <c r="J13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1087,76 +1078,76 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H17" s="6"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H27" s="6"/>
     </row>

</xml_diff>

<commit_message>
MAJ Objectif semaine prochaine Design
+ MAJ prog
</commit_message>
<xml_diff>
--- a/Objectif/Objectif.xlsx
+++ b/Objectif/Objectif.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
   <si>
     <t>DESIGN</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>Effets de particules</t>
+  </si>
+  <si>
+    <t>Objectif du 22/10/2014</t>
+  </si>
+  <si>
+    <t>Animation des collectibles (UNITY)</t>
+  </si>
+  <si>
+    <t>Jump mouvement</t>
   </si>
 </sst>
 </file>
@@ -297,7 +306,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -320,11 +329,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -335,6 +366,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,23 +972,71 @@
       </c>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
         <v>42</v>
       </c>
       <c r="H49" s="5"/>
     </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
         <v>43</v>
       </c>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
         <v>66</v>
       </c>
       <c r="H51" s="5"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>80</v>
+      </c>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H56" s="10"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>24</v>
+      </c>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>67</v>
+      </c>
+      <c r="H59" s="6"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" t="s">
+        <v>79</v>
+      </c>
+      <c r="H61" s="11"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H62" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -966,7 +1048,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1165,7 @@
       <c r="G15" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
@@ -1097,41 +1179,45 @@
       </c>
       <c r="H17" s="6"/>
     </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>45</v>
       </c>
-      <c r="G19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>74</v>
-      </c>
-      <c r="H21" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
         <v>75</v>
       </c>
-      <c r="H22" s="5"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>46</v>
       </c>
-      <c r="G24" t="s">
-        <v>51</v>
-      </c>
-      <c r="H24" s="6"/>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
@@ -1143,13 +1229,13 @@
       <c r="G26" t="s">
         <v>76</v>
       </c>
-      <c r="H26" s="6"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="6"/>
+      <c r="H27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Hit lvl 1 et maj objectif
</commit_message>
<xml_diff>
--- a/Objectif/Objectif.xlsx
+++ b/Objectif/Objectif.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -264,8 +264,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,7 +463,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -498,7 +497,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -674,14 +672,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
@@ -689,7 +687,7 @@
     <col min="7" max="7" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +704,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -720,7 +718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -729,48 +727,48 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="G7" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="G8" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="G9" t="s">
         <v>7</v>
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="G10" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="G11" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="C13" t="s">
         <v>17</v>
       </c>
@@ -779,42 +777,42 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="G14" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="G15" t="s">
         <v>20</v>
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="G16" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="G17" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="G18" t="s">
         <v>24</v>
       </c>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="C20" t="s">
         <v>25</v>
       </c>
@@ -823,26 +821,26 @@
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="G21" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="G22" t="s">
         <v>28</v>
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -850,12 +848,12 @@
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="C27" t="s">
         <v>3</v>
       </c>
@@ -864,49 +862,49 @@
       </c>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="G28" t="s">
         <v>30</v>
       </c>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="G29" t="s">
         <v>31</v>
       </c>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="G30" t="s">
         <v>32</v>
       </c>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="G31" t="s">
         <v>33</v>
       </c>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="G32" t="s">
         <v>34</v>
       </c>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8">
       <c r="G33" t="s">
         <v>35</v>
       </c>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:8">
       <c r="G34" t="s">
         <v>36</v>
       </c>
       <c r="H34" s="5"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:8">
       <c r="C36" t="s">
         <v>17</v>
       </c>
@@ -915,43 +913,43 @@
       </c>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:8">
       <c r="G37" t="s">
         <v>24</v>
       </c>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:8">
       <c r="G38" t="s">
         <v>37</v>
       </c>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:8">
       <c r="G39" t="s">
         <v>38</v>
       </c>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:8">
       <c r="G40" t="s">
         <v>39</v>
       </c>
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:8">
       <c r="G41" t="s">
         <v>67</v>
       </c>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H41" s="8"/>
+    </row>
+    <row r="42" spans="3:8">
       <c r="G42" t="s">
         <v>68</v>
       </c>
       <c r="H42" s="6"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:8">
       <c r="C46" t="s">
         <v>40</v>
       </c>
@@ -960,73 +958,73 @@
       </c>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:8">
       <c r="G47" t="s">
         <v>28</v>
       </c>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:8">
       <c r="G48" t="s">
         <v>41</v>
       </c>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="G49" t="s">
         <v>42</v>
       </c>
       <c r="H49" s="5"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="G50" t="s">
         <v>43</v>
       </c>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="G51" t="s">
         <v>66</v>
       </c>
       <c r="H51" s="5"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="C54" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="G55" t="s">
         <v>80</v>
       </c>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="H56" s="10"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="C57" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="G58" t="s">
         <v>24</v>
       </c>
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="G59" t="s">
         <v>67</v>
       </c>
-      <c r="H59" s="6"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="8"/>
+    </row>
+    <row r="61" spans="1:8">
       <c r="C61" t="s">
         <v>25</v>
       </c>
@@ -1035,7 +1033,7 @@
       </c>
       <c r="H61" s="11"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="H62" s="12"/>
     </row>
   </sheetData>
@@ -1044,21 +1042,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="39.140625" customWidth="1"/>
     <col min="10" max="10" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1075,7 +1073,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1092,7 +1090,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="C5" t="s">
         <v>44</v>
       </c>
@@ -1104,19 +1102,19 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="G6" t="s">
         <v>48</v>
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="G7" t="s">
         <v>53</v>
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="C9" t="s">
         <v>45</v>
       </c>
@@ -1128,13 +1126,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="G10" t="s">
         <v>50</v>
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="C12" t="s">
         <v>46</v>
       </c>
@@ -1146,7 +1144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="G13" t="s">
         <v>52</v>
       </c>
@@ -1155,7 +1153,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1167,71 +1165,71 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="G16" t="s">
         <v>71</v>
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8">
       <c r="G17" t="s">
         <v>69</v>
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8">
       <c r="G18" t="s">
         <v>51</v>
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8">
       <c r="C19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8">
       <c r="G20" t="s">
         <v>72</v>
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:8">
       <c r="G21" t="s">
         <v>73</v>
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:8">
       <c r="G22" t="s">
         <v>74</v>
       </c>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8">
       <c r="G23" t="s">
         <v>75</v>
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:8">
       <c r="C24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:8">
       <c r="G25" t="s">
         <v>52</v>
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:8">
       <c r="G26" t="s">
         <v>76</v>
       </c>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:8">
       <c r="G27" t="s">
         <v>77</v>
       </c>
@@ -1243,12 +1241,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Maj objectifs + fiche itération
</commit_message>
<xml_diff>
--- a/Objectif/Objectif.xlsx
+++ b/Objectif/Objectif.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="124">
   <si>
     <t>DESIGN</t>
   </si>
@@ -373,16 +373,38 @@
   </si>
   <si>
     <t>Image Licencié</t>
+  </si>
+  <si>
+    <t>Objectif du 12/10/2014</t>
+  </si>
+  <si>
+    <t>Mise en place des designs finaux</t>
+  </si>
+  <si>
+    <t>Animation des ennemis</t>
+  </si>
+  <si>
+    <t>Animation du background</t>
+  </si>
+  <si>
+    <t>VACANCE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -481,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -497,6 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D58" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,7 +1310,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
         <v>106</v>
       </c>
@@ -1299,7 +1322,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
         <v>107</v>
       </c>
@@ -1308,8 +1331,89 @@
         <v>117</v>
       </c>
     </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>3</v>
+      </c>
+      <c r="G85" t="s">
+        <v>113</v>
+      </c>
+      <c r="H85" s="8"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
+        <v>116</v>
+      </c>
+      <c r="H86" s="8"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
+        <v>104</v>
+      </c>
+      <c r="H87" s="6"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G88" t="s">
+        <v>120</v>
+      </c>
+      <c r="H88" s="6"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
+        <v>121</v>
+      </c>
+      <c r="H89" s="6"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>17</v>
+      </c>
+      <c r="G91" t="s">
+        <v>114</v>
+      </c>
+      <c r="H91" s="8"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
+        <v>115</v>
+      </c>
+      <c r="H92" s="8"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
+        <v>120</v>
+      </c>
+      <c r="H93" s="6"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
+        <v>121</v>
+      </c>
+      <c r="H94" s="6"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G95" t="s">
+        <v>122</v>
+      </c>
+      <c r="H95" s="15"/>
+    </row>
+    <row r="97" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>25</v>
+      </c>
+      <c r="G97" t="s">
+        <v>123</v>
+      </c>
+      <c r="H97" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Mise à jour objectif
Mis à jour.
</commit_message>
<xml_diff>
--- a/Objectif/Objectif.xlsx
+++ b/Objectif/Objectif.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="142">
   <si>
     <t>DESIGN</t>
   </si>
@@ -384,9 +384,6 @@
     <t>Animation du background</t>
   </si>
   <si>
-    <t>VACANCE</t>
-  </si>
-  <si>
     <t>Objectif du 5/11/2014</t>
   </si>
   <si>
@@ -402,7 +399,49 @@
     <t>Animations enemis</t>
   </si>
   <si>
-    <t>Repositionnement avec musique</t>
+    <t>VACANCES</t>
+  </si>
+  <si>
+    <t>Design plateforme, évolution journée</t>
+  </si>
+  <si>
+    <t>Destructible</t>
+  </si>
+  <si>
+    <t>Background, évolution journée</t>
+  </si>
+  <si>
+    <t>Avec Stan</t>
+  </si>
+  <si>
+    <t>Avec Ludo</t>
+  </si>
+  <si>
+    <t>Refait par Ludo</t>
+  </si>
+  <si>
+    <t>Fait par Ludo</t>
+  </si>
+  <si>
+    <t>Design fond de menu</t>
+  </si>
+  <si>
+    <t>Menu navigable au clavier</t>
+  </si>
+  <si>
+    <t>Crédits</t>
+  </si>
+  <si>
+    <t>Menu d'affichage touche</t>
+  </si>
+  <si>
+    <t>Correction de bug</t>
+  </si>
+  <si>
+    <t>Repositionnement musique (Checkpoint)</t>
+  </si>
+  <si>
+    <t>Camera</t>
   </si>
 </sst>
 </file>
@@ -841,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K97"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="K87" sqref="K87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,19 +1101,19 @@
       </c>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
         <v>35</v>
       </c>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
         <v>36</v>
       </c>
       <c r="H34" s="5"/>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>17</v>
       </c>
@@ -1083,43 +1122,49 @@
       </c>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
         <v>24</v>
       </c>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
         <v>37</v>
       </c>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
         <v>38</v>
       </c>
       <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
         <v>39</v>
       </c>
       <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
         <v>67</v>
       </c>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
         <v>68</v>
       </c>
       <c r="H42" s="6"/>
     </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>40</v>
       </c>
@@ -1131,13 +1176,13 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>28</v>
       </c>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
         <v>41</v>
       </c>
@@ -1267,6 +1312,9 @@
         <v>101</v>
       </c>
       <c r="H71" s="5"/>
+      <c r="K71" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="72" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
@@ -1358,13 +1406,13 @@
       <c r="G85" t="s">
         <v>112</v>
       </c>
-      <c r="H85" s="8"/>
+      <c r="H85" s="5"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
         <v>115</v>
       </c>
-      <c r="H86" s="8"/>
+      <c r="H86" s="5"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G87" t="s">
@@ -1382,49 +1430,73 @@
       <c r="G89" t="s">
         <v>120</v>
       </c>
-      <c r="H89" s="6"/>
+      <c r="H89" s="11"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
+        <v>128</v>
+      </c>
+      <c r="H90" s="13"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
-        <v>17</v>
-      </c>
       <c r="G91" t="s">
-        <v>113</v>
-      </c>
-      <c r="H91" s="8"/>
+        <v>129</v>
+      </c>
+      <c r="H91" s="13"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
-        <v>114</v>
-      </c>
-      <c r="H92" s="8"/>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G93" t="s">
-        <v>119</v>
-      </c>
-      <c r="H93" s="6"/>
+        <v>130</v>
+      </c>
+      <c r="H92" s="13"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>17</v>
+      </c>
       <c r="G94" t="s">
-        <v>120</v>
-      </c>
-      <c r="H94" s="6"/>
+        <v>113</v>
+      </c>
+      <c r="H94" s="5"/>
+      <c r="K94" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
+        <v>114</v>
+      </c>
+      <c r="H95" s="5"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
+        <v>119</v>
+      </c>
+      <c r="H96" s="8"/>
+    </row>
+    <row r="97" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
+        <v>120</v>
+      </c>
+      <c r="H97" s="8"/>
+      <c r="K97" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="98" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
         <v>121</v>
       </c>
-      <c r="H95" s="15"/>
-    </row>
-    <row r="97" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
+      <c r="H98" s="15"/>
+    </row>
+    <row r="100" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
         <v>25</v>
       </c>
-      <c r="G97" t="s">
-        <v>122</v>
-      </c>
-      <c r="H97" s="5"/>
+      <c r="G100" t="s">
+        <v>127</v>
+      </c>
+      <c r="H100" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1434,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,7 +1770,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C40" t="s">
         <v>44</v>
@@ -1770,36 +1842,72 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C53" t="s">
         <v>44</v>
       </c>
       <c r="G53" t="s">
-        <v>125</v>
-      </c>
-      <c r="H53" s="6"/>
+        <v>124</v>
+      </c>
+      <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H54" s="6"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>141</v>
+      </c>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
         <v>45</v>
       </c>
-      <c r="G56" t="s">
-        <v>126</v>
-      </c>
-      <c r="H56" s="6"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>140</v>
+      </c>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>135</v>
+      </c>
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>136</v>
+      </c>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>137</v>
+      </c>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>138</v>
+      </c>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>139</v>
+      </c>
+      <c r="H63" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>